<commit_message>
modulo fia + modifiche lista utenti in Evento
</commit_message>
<xml_diff>
--- a/doc/deliverables/Matrice-Tracciabilità.xlsx
+++ b/doc/deliverables/Matrice-Tracciabilità.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enzuc\Desktop\Università\Terzo anno\Primo Semestre\Ingegneria del software\Progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arusc\IdeaProjects\AVAfieldProject\doc\deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEAF9CD-9435-4B48-90C9-274CCCCD8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F5A38E-4793-400B-952C-0FC87F4EE0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -724,22 +724,22 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -747,7 +747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -755,7 +755,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -810,7 +810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -830,7 +830,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -856,7 +856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -876,7 +876,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -896,7 +896,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -922,7 +922,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -951,7 +951,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -980,7 +980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>

</xml_diff>